<commit_message>
made plots for time series data
</commit_message>
<xml_diff>
--- a/2019_nCoV_time_series.xlsx
+++ b/2019_nCoV_time_series.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="124">
   <si>
     <t>Province/State</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>2/5/2020 9:00 AM</t>
+  </si>
+  <si>
+    <t>2/6/2020 2:20 PM</t>
   </si>
   <si>
     <t>Anhui</t>
@@ -742,13 +745,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG68"/>
+  <dimension ref="A1:AH68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:34">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,16 +851,19 @@
       <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D2">
         <v>31.82571</v>
@@ -949,16 +955,19 @@
       <c r="AG2">
         <v>530</v>
       </c>
+      <c r="AH2">
+        <v>591</v>
+      </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:34">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D3">
         <v>40.18238</v>
@@ -1050,16 +1059,19 @@
       <c r="AG3">
         <v>253</v>
       </c>
+      <c r="AH3">
+        <v>274</v>
+      </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:34">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D4">
         <v>30.05718</v>
@@ -1151,16 +1163,19 @@
       <c r="AG4">
         <v>376</v>
       </c>
+      <c r="AH4">
+        <v>400</v>
+      </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:34">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>26.07783</v>
@@ -1252,16 +1267,19 @@
       <c r="AG5">
         <v>205</v>
       </c>
+      <c r="AH5">
+        <v>215</v>
+      </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:34">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D6">
         <v>36.0611</v>
@@ -1353,16 +1371,19 @@
       <c r="AG6">
         <v>57</v>
       </c>
+      <c r="AH6">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:34">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>23.33841</v>
@@ -1454,16 +1475,19 @@
       <c r="AG7">
         <v>895</v>
       </c>
+      <c r="AH7">
+        <v>970</v>
+      </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:34">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <v>23.82908</v>
@@ -1555,16 +1579,19 @@
       <c r="AG8">
         <v>150</v>
       </c>
+      <c r="AH8">
+        <v>168</v>
+      </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:34">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D9">
         <v>26.81536</v>
@@ -1656,16 +1683,19 @@
       <c r="AG9">
         <v>64</v>
       </c>
+      <c r="AH9">
+        <v>71</v>
+      </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:34">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D10">
         <v>19.19673</v>
@@ -1757,16 +1787,19 @@
       <c r="AG10">
         <v>91</v>
       </c>
+      <c r="AH10">
+        <v>106</v>
+      </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:34">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D11">
         <v>38.0428</v>
@@ -1858,16 +1891,19 @@
       <c r="AG11">
         <v>135</v>
       </c>
+      <c r="AH11">
+        <v>157</v>
+      </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:34">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D12">
         <v>47.862</v>
@@ -1959,16 +1995,19 @@
       <c r="AG12">
         <v>190</v>
       </c>
+      <c r="AH12">
+        <v>227</v>
+      </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:34">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>33.88202</v>
@@ -2060,16 +2099,19 @@
       <c r="AG13">
         <v>764</v>
       </c>
+      <c r="AH13">
+        <v>851</v>
+      </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:34">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>30.97564</v>
@@ -2161,16 +2203,19 @@
       <c r="AG14">
         <v>16678</v>
       </c>
+      <c r="AH14">
+        <v>19665</v>
+      </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:34">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>27.61041</v>
@@ -2262,16 +2307,19 @@
       <c r="AG15">
         <v>661</v>
       </c>
+      <c r="AH15">
+        <v>711</v>
+      </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:34">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D16">
         <v>44.09448</v>
@@ -2363,16 +2411,19 @@
       <c r="AG16">
         <v>42</v>
       </c>
+      <c r="AH16">
+        <v>46</v>
+      </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:34">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D17">
         <v>32.97027</v>
@@ -2464,16 +2515,19 @@
       <c r="AG17">
         <v>341</v>
       </c>
+      <c r="AH17">
+        <v>373</v>
+      </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:34">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>27.61401</v>
@@ -2565,16 +2619,19 @@
       <c r="AG18">
         <v>548</v>
       </c>
+      <c r="AH18">
+        <v>600</v>
+      </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:34">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D19">
         <v>43.66657</v>
@@ -2666,16 +2723,19 @@
       <c r="AG19">
         <v>54</v>
       </c>
+      <c r="AH19">
+        <v>59</v>
+      </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:34">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <v>41.29284</v>
@@ -2767,16 +2827,19 @@
       <c r="AG20">
         <v>88</v>
       </c>
+      <c r="AH20">
+        <v>94</v>
+      </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:34">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D21">
         <v>37.26923</v>
@@ -2868,16 +2931,19 @@
       <c r="AG21">
         <v>34</v>
       </c>
+      <c r="AH21">
+        <v>40</v>
+      </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:34">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22">
         <v>35.65945</v>
@@ -2969,16 +3035,19 @@
       <c r="AG22">
         <v>17</v>
       </c>
+      <c r="AH22">
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:34">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D23">
         <v>35.19165</v>
@@ -3070,16 +3139,19 @@
       <c r="AG23">
         <v>165</v>
       </c>
+      <c r="AH23">
+        <v>173</v>
+      </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:34">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D24">
         <v>36.34377</v>
@@ -3171,16 +3243,19 @@
       <c r="AG24">
         <v>307</v>
       </c>
+      <c r="AH24">
+        <v>347</v>
+      </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:34">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25">
         <v>31.20327</v>
@@ -3272,16 +3347,19 @@
       <c r="AG25">
         <v>243</v>
       </c>
+      <c r="AH25">
+        <v>257</v>
+      </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:34">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D26">
         <v>37.57769</v>
@@ -3373,16 +3451,19 @@
       <c r="AG26">
         <v>81</v>
       </c>
+      <c r="AH26">
+        <v>90</v>
+      </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:34">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D27">
         <v>30.61714</v>
@@ -3474,16 +3555,19 @@
       <c r="AG27">
         <v>301</v>
       </c>
+      <c r="AH27">
+        <v>321</v>
+      </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:34">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D28">
         <v>39.29362</v>
@@ -3575,16 +3659,19 @@
       <c r="AG28">
         <v>69</v>
       </c>
+      <c r="AH28">
+        <v>78</v>
+      </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:34">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D29">
         <v>30.1534</v>
@@ -3676,16 +3763,19 @@
       <c r="AG29">
         <v>1</v>
       </c>
+      <c r="AH29">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:34">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D30">
         <v>41.11981</v>
@@ -3777,16 +3867,19 @@
       <c r="AG30">
         <v>32</v>
       </c>
+      <c r="AH30">
+        <v>36</v>
+      </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:34">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D31">
         <v>24.97411</v>
@@ -3878,16 +3971,19 @@
       <c r="AG31">
         <v>124</v>
       </c>
+      <c r="AH31">
+        <v>133</v>
+      </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:34">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D32">
         <v>29.18251</v>
@@ -3979,13 +4075,16 @@
       <c r="AG32">
         <v>895</v>
       </c>
+      <c r="AH32">
+        <v>954</v>
+      </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:34">
       <c r="B33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D33">
         <v>13.7563</v>
@@ -4077,13 +4176,16 @@
       <c r="AG33">
         <v>25</v>
       </c>
+      <c r="AH33">
+        <v>25</v>
+      </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:34">
       <c r="B34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D34">
         <v>35.6762</v>
@@ -4175,13 +4277,16 @@
       <c r="AG34">
         <v>22</v>
       </c>
+      <c r="AH34">
+        <v>45</v>
+      </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:34">
       <c r="B35" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D35">
         <v>37.5665</v>
@@ -4273,16 +4378,19 @@
       <c r="AG35">
         <v>16</v>
       </c>
+      <c r="AH35">
+        <v>23</v>
+      </c>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:34">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D36">
         <v>23.6978</v>
@@ -4374,16 +4482,19 @@
       <c r="AG36">
         <v>11</v>
       </c>
+      <c r="AH36">
+        <v>16</v>
+      </c>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:34">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D37">
         <v>47.7511</v>
@@ -4475,16 +4586,19 @@
       <c r="AG37">
         <v>1</v>
       </c>
+      <c r="AH37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:34">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D38">
         <v>40.6331</v>
@@ -4576,16 +4690,19 @@
       <c r="AG38">
         <v>2</v>
       </c>
+      <c r="AH38">
+        <v>2</v>
+      </c>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:34">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D39">
         <v>36.7783</v>
@@ -4677,16 +4794,19 @@
       <c r="AG39">
         <v>6</v>
       </c>
+      <c r="AH39">
+        <v>6</v>
+      </c>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:34">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D40">
         <v>34.0489</v>
@@ -4778,16 +4898,19 @@
       <c r="AG40">
         <v>1</v>
       </c>
+      <c r="AH40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:34">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D41">
         <v>22.1987</v>
@@ -4879,16 +5002,19 @@
       <c r="AG41">
         <v>10</v>
       </c>
+      <c r="AH41">
+        <v>10</v>
+      </c>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:34">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D42">
         <v>22.3193</v>
@@ -4980,13 +5106,16 @@
       <c r="AG42">
         <v>21</v>
       </c>
+      <c r="AH42">
+        <v>24</v>
+      </c>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:34">
       <c r="B43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D43">
         <v>1.3521</v>
@@ -5078,13 +5207,16 @@
       <c r="AG43">
         <v>24</v>
       </c>
+      <c r="AH43">
+        <v>28</v>
+      </c>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:34">
       <c r="B44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D44">
         <v>21.0278</v>
@@ -5176,13 +5308,16 @@
       <c r="AG44">
         <v>8</v>
       </c>
+      <c r="AH44">
+        <v>10</v>
+      </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:34">
       <c r="B45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D45">
         <v>46.2276</v>
@@ -5274,13 +5409,16 @@
       <c r="AG45">
         <v>6</v>
       </c>
+      <c r="AH45">
+        <v>6</v>
+      </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:34">
       <c r="B46" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D46">
         <v>28.3949</v>
@@ -5372,13 +5510,16 @@
       <c r="AG46">
         <v>1</v>
       </c>
+      <c r="AH46">
+        <v>1</v>
+      </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:34">
       <c r="B47" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D47">
         <v>4.2105</v>
@@ -5470,16 +5611,19 @@
       <c r="AG47">
         <v>10</v>
       </c>
+      <c r="AH47">
+        <v>12</v>
+      </c>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:34">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D48">
         <v>43.6532</v>
@@ -5571,16 +5715,19 @@
       <c r="AG48">
         <v>3</v>
       </c>
+      <c r="AH48">
+        <v>3</v>
+      </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:34">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D49">
         <v>49.2827</v>
@@ -5672,16 +5819,19 @@
       <c r="AG49">
         <v>1</v>
       </c>
+      <c r="AH49">
+        <v>2</v>
+      </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:34">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D50">
         <v>-33.8688</v>
@@ -5773,16 +5923,19 @@
       <c r="AG50">
         <v>4</v>
       </c>
+      <c r="AH50">
+        <v>4</v>
+      </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:34">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D51">
         <v>-37.8136</v>
@@ -5874,16 +6027,19 @@
       <c r="AG51">
         <v>4</v>
       </c>
+      <c r="AH51">
+        <v>4</v>
+      </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:34">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D52">
         <v>-27.4698</v>
@@ -5975,13 +6131,16 @@
       <c r="AG52">
         <v>3</v>
       </c>
+      <c r="AH52">
+        <v>4</v>
+      </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:34">
       <c r="B53" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D53">
         <v>12.5657</v>
@@ -6073,13 +6232,16 @@
       <c r="AG53">
         <v>1</v>
       </c>
+      <c r="AH53">
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:34">
       <c r="B54" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54">
         <v>7.8731</v>
@@ -6171,13 +6333,16 @@
       <c r="AG54">
         <v>1</v>
       </c>
+      <c r="AH54">
+        <v>1</v>
+      </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:34">
       <c r="B55" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D55">
         <v>51.1657</v>
@@ -6269,13 +6434,16 @@
       <c r="AG55">
         <v>12</v>
       </c>
+      <c r="AH55">
+        <v>12</v>
+      </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:34">
       <c r="B56" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D56">
         <v>61.9241</v>
@@ -6367,13 +6535,16 @@
       <c r="AG56">
         <v>1</v>
       </c>
+      <c r="AH56">
+        <v>1</v>
+      </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:34">
       <c r="B57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D57">
         <v>23.4241</v>
@@ -6465,13 +6636,16 @@
       <c r="AG57">
         <v>5</v>
       </c>
+      <c r="AH57">
+        <v>5</v>
+      </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:34">
       <c r="B58" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D58">
         <v>12.8797</v>
@@ -6563,13 +6737,16 @@
       <c r="AG58">
         <v>2</v>
       </c>
+      <c r="AH58">
+        <v>2</v>
+      </c>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:34">
       <c r="B59" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D59">
         <v>20.5937</v>
@@ -6661,13 +6838,16 @@
       <c r="AG59">
         <v>3</v>
       </c>
+      <c r="AH59">
+        <v>3</v>
+      </c>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:34">
       <c r="B60" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C60" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D60">
         <v>41.8719</v>
@@ -6759,13 +6939,16 @@
       <c r="AG60">
         <v>2</v>
       </c>
+      <c r="AH60">
+        <v>2</v>
+      </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:34">
       <c r="B61" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D61">
         <v>55.3781</v>
@@ -6857,13 +7040,16 @@
       <c r="AG61">
         <v>2</v>
       </c>
+      <c r="AH61">
+        <v>2</v>
+      </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:34">
       <c r="B62" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D62">
         <v>61.524</v>
@@ -6955,13 +7141,16 @@
       <c r="AG62">
         <v>2</v>
       </c>
+      <c r="AH62">
+        <v>2</v>
+      </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:34">
       <c r="B63" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D63">
         <v>60.1282</v>
@@ -7053,13 +7242,16 @@
       <c r="AG63">
         <v>1</v>
       </c>
+      <c r="AH63">
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:34">
       <c r="B64" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D64">
         <v>40.4637</v>
@@ -7151,16 +7343,19 @@
       <c r="AG64">
         <v>1</v>
       </c>
+      <c r="AH64">
+        <v>1</v>
+      </c>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:34">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D65">
         <v>-34.9285</v>
@@ -7252,16 +7447,19 @@
       <c r="AG65">
         <v>2</v>
       </c>
+      <c r="AH65">
+        <v>2</v>
+      </c>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:34">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D66">
         <v>42.3601</v>
@@ -7353,13 +7551,16 @@
       <c r="AG66">
         <v>1</v>
       </c>
+      <c r="AH66">
+        <v>1</v>
+      </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:34">
       <c r="B67" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D67">
         <v>50.5039</v>
@@ -7451,16 +7652,19 @@
       <c r="AG67">
         <v>1</v>
       </c>
+      <c r="AH67">
+        <v>1</v>
+      </c>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:34">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D68">
         <v>43.0731</v>
@@ -7551,6 +7755,9 @@
       </c>
       <c r="AG68">
         <v>0</v>
+      </c>
+      <c r="AH68">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -7560,13 +7767,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF68"/>
+  <dimension ref="A1:AG68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7574,7 +7781,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -7663,16 +7870,19 @@
       <c r="AF1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AG1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D2">
         <v>31.82571</v>
@@ -7761,16 +7971,19 @@
       <c r="AF2">
         <v>23</v>
       </c>
+      <c r="AG2">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D3">
         <v>40.18238</v>
@@ -7859,16 +8072,19 @@
       <c r="AF3">
         <v>24</v>
       </c>
+      <c r="AG3">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D4">
         <v>30.05718</v>
@@ -7957,16 +8173,19 @@
       <c r="AF4">
         <v>15</v>
       </c>
+      <c r="AG4">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>26.07783</v>
@@ -8055,16 +8274,19 @@
       <c r="AF5">
         <v>11</v>
       </c>
+      <c r="AG5">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D6">
         <v>36.0611</v>
@@ -8153,16 +8375,19 @@
       <c r="AF6">
         <v>4</v>
       </c>
+      <c r="AG6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>23.33841</v>
@@ -8251,16 +8476,19 @@
       <c r="AF7">
         <v>49</v>
       </c>
+      <c r="AG7">
+        <v>69</v>
+      </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <v>23.82908</v>
@@ -8349,16 +8577,19 @@
       <c r="AF8">
         <v>13</v>
       </c>
+      <c r="AG8">
+        <v>14</v>
+      </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D9">
         <v>26.81536</v>
@@ -8447,16 +8678,19 @@
       <c r="AF9">
         <v>9</v>
       </c>
+      <c r="AG9">
+        <v>6</v>
+      </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D10">
         <v>19.19673</v>
@@ -8545,16 +8779,19 @@
       <c r="AF10">
         <v>5</v>
       </c>
+      <c r="AG10">
+        <v>8</v>
+      </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D11">
         <v>38.0428</v>
@@ -8643,16 +8880,19 @@
       <c r="AF11">
         <v>6</v>
       </c>
+      <c r="AG11">
+        <v>13</v>
+      </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D12">
         <v>47.862</v>
@@ -8741,16 +8981,19 @@
       <c r="AF12">
         <v>7</v>
       </c>
+      <c r="AG12">
+        <v>8</v>
+      </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>33.88202</v>
@@ -8839,16 +9082,19 @@
       <c r="AF13">
         <v>47</v>
       </c>
+      <c r="AG13">
+        <v>56</v>
+      </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>30.97564</v>
@@ -8937,16 +9183,19 @@
       <c r="AF14">
         <v>537</v>
       </c>
+      <c r="AG14">
+        <v>712</v>
+      </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>27.61041</v>
@@ -9035,16 +9284,19 @@
       <c r="AF15">
         <v>53</v>
       </c>
+      <c r="AG15">
+        <v>54</v>
+      </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D16">
         <v>44.09448</v>
@@ -9133,16 +9385,19 @@
       <c r="AF16">
         <v>3</v>
       </c>
+      <c r="AG16">
+        <v>4</v>
+      </c>
     </row>
-    <row r="17" spans="1:32">
+    <row r="17" spans="1:33">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D17">
         <v>32.97027</v>
@@ -9231,16 +9486,19 @@
       <c r="AF17">
         <v>23</v>
       </c>
+      <c r="AG17">
+        <v>34</v>
+      </c>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:33">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>27.61401</v>
@@ -9329,16 +9587,19 @@
       <c r="AF18">
         <v>27</v>
       </c>
+      <c r="AG18">
+        <v>37</v>
+      </c>
     </row>
-    <row r="19" spans="1:32">
+    <row r="19" spans="1:33">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D19">
         <v>43.66657</v>
@@ -9427,16 +9688,19 @@
       <c r="AF19">
         <v>2</v>
       </c>
+      <c r="AG19">
+        <v>4</v>
+      </c>
     </row>
-    <row r="20" spans="1:32">
+    <row r="20" spans="1:33">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <v>41.29284</v>
@@ -9525,16 +9789,19 @@
       <c r="AF20">
         <v>4</v>
       </c>
+      <c r="AG20">
+        <v>5</v>
+      </c>
     </row>
-    <row r="21" spans="1:32">
+    <row r="21" spans="1:33">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D21">
         <v>37.26923</v>
@@ -9623,16 +9890,19 @@
       <c r="AF21">
         <v>1</v>
       </c>
+      <c r="AG21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:32">
+    <row r="22" spans="1:33">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22">
         <v>35.65945</v>
@@ -9721,16 +9991,19 @@
       <c r="AF22">
         <v>3</v>
       </c>
+      <c r="AG22">
+        <v>3</v>
+      </c>
     </row>
-    <row r="23" spans="1:32">
+    <row r="23" spans="1:33">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D23">
         <v>35.19165</v>
@@ -9819,16 +10092,19 @@
       <c r="AF23">
         <v>6</v>
       </c>
+      <c r="AG23">
+        <v>9</v>
+      </c>
     </row>
-    <row r="24" spans="1:32">
+    <row r="24" spans="1:33">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D24">
         <v>36.34377</v>
@@ -9917,16 +10193,19 @@
       <c r="AF24">
         <v>15</v>
       </c>
+      <c r="AG24">
+        <v>27</v>
+      </c>
     </row>
-    <row r="25" spans="1:32">
+    <row r="25" spans="1:33">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25">
         <v>31.20327</v>
@@ -10015,16 +10294,19 @@
       <c r="AF25">
         <v>15</v>
       </c>
+      <c r="AG25">
+        <v>25</v>
+      </c>
     </row>
-    <row r="26" spans="1:32">
+    <row r="26" spans="1:33">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D26">
         <v>37.57769</v>
@@ -10113,16 +10395,19 @@
       <c r="AF26">
         <v>4</v>
       </c>
+      <c r="AG26">
+        <v>12</v>
+      </c>
     </row>
-    <row r="27" spans="1:32">
+    <row r="27" spans="1:33">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D27">
         <v>30.61714</v>
@@ -10211,16 +10496,19 @@
       <c r="AF27">
         <v>24</v>
       </c>
+      <c r="AG27">
+        <v>31</v>
+      </c>
     </row>
-    <row r="28" spans="1:32">
+    <row r="28" spans="1:33">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D28">
         <v>39.29362</v>
@@ -10309,16 +10597,19 @@
       <c r="AF28">
         <v>2</v>
       </c>
+      <c r="AG28">
+        <v>2</v>
+      </c>
     </row>
-    <row r="29" spans="1:32">
+    <row r="29" spans="1:33">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D29">
         <v>30.1534</v>
@@ -10407,16 +10698,19 @@
       <c r="AF29">
         <v>0</v>
       </c>
+      <c r="AG29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:32">
+    <row r="30" spans="1:33">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D30">
         <v>41.11981</v>
@@ -10505,16 +10799,19 @@
       <c r="AF30">
         <v>0</v>
       </c>
+      <c r="AG30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:32">
+    <row r="31" spans="1:33">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D31">
         <v>24.97411</v>
@@ -10603,16 +10900,19 @@
       <c r="AF31">
         <v>5</v>
       </c>
+      <c r="AG31">
+        <v>7</v>
+      </c>
     </row>
-    <row r="32" spans="1:32">
+    <row r="32" spans="1:33">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D32">
         <v>29.18251</v>
@@ -10699,18 +10999,21 @@
         <v>63</v>
       </c>
       <c r="AF32">
-        <v>7</v>
+        <v>78</v>
+      </c>
+      <c r="AG32">
+        <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:32">
+    <row r="33" spans="1:33">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D33">
         <v>22.3193</v>
@@ -10799,16 +11102,19 @@
       <c r="AF33">
         <v>0</v>
       </c>
+      <c r="AG33">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:32">
+    <row r="34" spans="1:33">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D34">
         <v>22.1987</v>
@@ -10897,16 +11203,19 @@
       <c r="AF34">
         <v>0</v>
       </c>
+      <c r="AG34">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:32">
+    <row r="35" spans="1:33">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D35">
         <v>23.6978</v>
@@ -10995,16 +11304,19 @@
       <c r="AF35">
         <v>0</v>
       </c>
+      <c r="AG35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:32">
+    <row r="36" spans="1:33">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D36">
         <v>47.7511</v>
@@ -11093,16 +11405,19 @@
       <c r="AF36">
         <v>0</v>
       </c>
+      <c r="AG36">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:32">
+    <row r="37" spans="1:33">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D37">
         <v>40.6331</v>
@@ -11191,16 +11506,19 @@
       <c r="AF37">
         <v>0</v>
       </c>
+      <c r="AG37">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:32">
+    <row r="38" spans="1:33">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D38">
         <v>36.7783</v>
@@ -11289,16 +11607,19 @@
       <c r="AF38">
         <v>0</v>
       </c>
+      <c r="AG38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:32">
+    <row r="39" spans="1:33">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D39">
         <v>34.0489</v>
@@ -11387,13 +11708,16 @@
       <c r="AF39">
         <v>0</v>
       </c>
+      <c r="AG39">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:32">
+    <row r="40" spans="1:33">
       <c r="B40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D40">
         <v>35.6762</v>
@@ -11482,13 +11806,16 @@
       <c r="AF40">
         <v>1</v>
       </c>
+      <c r="AG40">
+        <v>1</v>
+      </c>
     </row>
-    <row r="41" spans="1:32">
+    <row r="41" spans="1:33">
       <c r="B41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D41">
         <v>13.7563</v>
@@ -11577,13 +11904,16 @@
       <c r="AF41">
         <v>5</v>
       </c>
+      <c r="AG41">
+        <v>5</v>
+      </c>
     </row>
-    <row r="42" spans="1:32">
+    <row r="42" spans="1:33">
       <c r="B42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D42">
         <v>37.5665</v>
@@ -11672,13 +12002,16 @@
       <c r="AF42">
         <v>0</v>
       </c>
+      <c r="AG42">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:32">
+    <row r="43" spans="1:33">
       <c r="B43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D43">
         <v>1.3521</v>
@@ -11767,13 +12100,16 @@
       <c r="AF43">
         <v>0</v>
       </c>
+      <c r="AG43">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:32">
+    <row r="44" spans="1:33">
       <c r="B44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D44">
         <v>21.0278</v>
@@ -11862,13 +12198,16 @@
       <c r="AF44">
         <v>1</v>
       </c>
+      <c r="AG44">
+        <v>1</v>
+      </c>
     </row>
-    <row r="45" spans="1:32">
+    <row r="45" spans="1:33">
       <c r="B45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D45">
         <v>46.2276</v>
@@ -11957,13 +12296,16 @@
       <c r="AF45">
         <v>0</v>
       </c>
+      <c r="AG45">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:32">
+    <row r="46" spans="1:33">
       <c r="B46" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D46">
         <v>28.3949</v>
@@ -12052,13 +12394,16 @@
       <c r="AF46">
         <v>0</v>
       </c>
+      <c r="AG46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:32">
+    <row r="47" spans="1:33">
       <c r="B47" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D47">
         <v>4.2105</v>
@@ -12147,16 +12492,19 @@
       <c r="AF47">
         <v>0</v>
       </c>
+      <c r="AG47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:32">
+    <row r="48" spans="1:33">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D48">
         <v>43.6532</v>
@@ -12245,16 +12593,19 @@
       <c r="AF48">
         <v>0</v>
       </c>
+      <c r="AG48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:32">
+    <row r="49" spans="1:33">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D49">
         <v>49.2827</v>
@@ -12343,16 +12694,19 @@
       <c r="AF49">
         <v>0</v>
       </c>
+      <c r="AG49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:32">
+    <row r="50" spans="1:33">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D50">
         <v>-33.8688</v>
@@ -12441,16 +12795,19 @@
       <c r="AF50">
         <v>2</v>
       </c>
+      <c r="AG50">
+        <v>2</v>
+      </c>
     </row>
-    <row r="51" spans="1:32">
+    <row r="51" spans="1:33">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D51">
         <v>-37.8136</v>
@@ -12539,16 +12896,19 @@
       <c r="AF51">
         <v>0</v>
       </c>
+      <c r="AG51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:32">
+    <row r="52" spans="1:33">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D52">
         <v>-27.4698</v>
@@ -12637,13 +12997,16 @@
       <c r="AF52">
         <v>0</v>
       </c>
+      <c r="AG52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:32">
+    <row r="53" spans="1:33">
       <c r="B53" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D53">
         <v>12.5657</v>
@@ -12732,13 +13095,16 @@
       <c r="AF53">
         <v>0</v>
       </c>
+      <c r="AG53">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:32">
+    <row r="54" spans="1:33">
       <c r="B54" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54">
         <v>7.8731</v>
@@ -12827,16 +13193,19 @@
       <c r="AF54">
         <v>0</v>
       </c>
+      <c r="AG54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:32">
+    <row r="55" spans="1:33">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D55">
         <v>51.1657</v>
@@ -12925,13 +13294,16 @@
       <c r="AF55">
         <v>0</v>
       </c>
+      <c r="AG55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:32">
+    <row r="56" spans="1:33">
       <c r="B56" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D56">
         <v>61.9241</v>
@@ -13020,13 +13392,16 @@
       <c r="AF56">
         <v>0</v>
       </c>
+      <c r="AG56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:32">
+    <row r="57" spans="1:33">
       <c r="B57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D57">
         <v>23.4241</v>
@@ -13115,13 +13490,16 @@
       <c r="AF57">
         <v>0</v>
       </c>
+      <c r="AG57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:32">
+    <row r="58" spans="1:33">
       <c r="B58" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D58">
         <v>12.8797</v>
@@ -13210,13 +13588,16 @@
       <c r="AF58">
         <v>0</v>
       </c>
+      <c r="AG58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:32">
+    <row r="59" spans="1:33">
       <c r="B59" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D59">
         <v>20.5937</v>
@@ -13305,13 +13686,16 @@
       <c r="AF59">
         <v>0</v>
       </c>
+      <c r="AG59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:32">
+    <row r="60" spans="1:33">
       <c r="B60" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C60" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D60">
         <v>41.8719</v>
@@ -13400,13 +13784,16 @@
       <c r="AF60">
         <v>0</v>
       </c>
+      <c r="AG60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:32">
+    <row r="61" spans="1:33">
       <c r="B61" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D61">
         <v>55.3781</v>
@@ -13495,13 +13882,16 @@
       <c r="AF61">
         <v>0</v>
       </c>
+      <c r="AG61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:32">
+    <row r="62" spans="1:33">
       <c r="B62" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D62">
         <v>61.524</v>
@@ -13590,13 +13980,16 @@
       <c r="AF62">
         <v>0</v>
       </c>
+      <c r="AG62">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:32">
+    <row r="63" spans="1:33">
       <c r="B63" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D63">
         <v>60.1282</v>
@@ -13685,13 +14078,16 @@
       <c r="AF63">
         <v>0</v>
       </c>
+      <c r="AG63">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:32">
+    <row r="64" spans="1:33">
       <c r="B64" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D64">
         <v>40.4637</v>
@@ -13780,16 +14176,19 @@
       <c r="AF64">
         <v>0</v>
       </c>
+      <c r="AG64">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:32">
+    <row r="65" spans="1:33">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D65">
         <v>-34.9285</v>
@@ -13878,16 +14277,19 @@
       <c r="AF65">
         <v>0</v>
       </c>
+      <c r="AG65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:32">
+    <row r="66" spans="1:33">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D66">
         <v>42.3601</v>
@@ -13976,13 +14378,16 @@
       <c r="AF66">
         <v>0</v>
       </c>
+      <c r="AG66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:32">
+    <row r="67" spans="1:33">
       <c r="B67" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D67">
         <v>50.5039</v>
@@ -14071,16 +14476,19 @@
       <c r="AF67">
         <v>0</v>
       </c>
+      <c r="AG67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:32">
+    <row r="68" spans="1:33">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D68">
         <v>43.0731</v>
@@ -14167,6 +14575,9 @@
         <v>0</v>
       </c>
       <c r="AF68">
+        <v>0</v>
+      </c>
+      <c r="AG68">
         <v>0</v>
       </c>
     </row>
@@ -14177,13 +14588,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD68"/>
+  <dimension ref="A1:AE68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14191,7 +14602,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -14274,16 +14685,19 @@
       <c r="AD1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AE1" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D2">
         <v>31.82571</v>
@@ -14366,16 +14780,19 @@
       <c r="AD2">
         <v>0</v>
       </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D3">
         <v>40.18238</v>
@@ -14458,16 +14875,19 @@
       <c r="AD3">
         <v>1</v>
       </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D4">
         <v>30.05718</v>
@@ -14550,16 +14970,19 @@
       <c r="AD4">
         <v>2</v>
       </c>
+      <c r="AE4">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>26.07783</v>
@@ -14642,16 +15065,19 @@
       <c r="AD5">
         <v>0</v>
       </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D6">
         <v>36.0611</v>
@@ -14734,16 +15160,19 @@
       <c r="AD6">
         <v>0</v>
       </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>23.33841</v>
@@ -14826,16 +15255,19 @@
       <c r="AD7">
         <v>0</v>
       </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D8">
         <v>23.82908</v>
@@ -14918,16 +15350,19 @@
       <c r="AD8">
         <v>0</v>
       </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D9">
         <v>26.81536</v>
@@ -15010,16 +15445,19 @@
       <c r="AD9">
         <v>1</v>
       </c>
+      <c r="AE9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D10">
         <v>19.19673</v>
@@ -15102,16 +15540,19 @@
       <c r="AD10">
         <v>1</v>
       </c>
+      <c r="AE10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D11">
         <v>38.0428</v>
@@ -15194,16 +15635,19 @@
       <c r="AD11">
         <v>1</v>
       </c>
+      <c r="AE11">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D12">
         <v>47.862</v>
@@ -15286,16 +15730,19 @@
       <c r="AD12">
         <v>2</v>
       </c>
+      <c r="AE12">
+        <v>3</v>
+      </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D13">
         <v>33.88202</v>
@@ -15378,16 +15825,19 @@
       <c r="AD13">
         <v>2</v>
       </c>
+      <c r="AE13">
+        <v>2</v>
+      </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>30.97564</v>
@@ -15470,16 +15920,19 @@
       <c r="AD14">
         <v>479</v>
       </c>
+      <c r="AE14">
+        <v>549</v>
+      </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>27.61041</v>
@@ -15562,16 +16015,19 @@
       <c r="AD15">
         <v>0</v>
       </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D16">
         <v>44.09448</v>
@@ -15654,16 +16110,19 @@
       <c r="AD16">
         <v>0</v>
       </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D17">
         <v>32.97027</v>
@@ -15746,16 +16205,19 @@
       <c r="AD17">
         <v>0</v>
       </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>27.61401</v>
@@ -15838,16 +16300,19 @@
       <c r="AD18">
         <v>0</v>
       </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D19">
         <v>43.66657</v>
@@ -15930,16 +16395,19 @@
       <c r="AD19">
         <v>0</v>
       </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <v>41.29284</v>
@@ -16022,16 +16490,19 @@
       <c r="AD20">
         <v>0</v>
       </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D21">
         <v>37.26923</v>
@@ -16114,16 +16585,19 @@
       <c r="AD21">
         <v>0</v>
       </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D22">
         <v>35.65945</v>
@@ -16206,16 +16680,19 @@
       <c r="AD22">
         <v>0</v>
       </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D23">
         <v>35.19165</v>
@@ -16298,16 +16775,19 @@
       <c r="AD23">
         <v>0</v>
       </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D24">
         <v>36.34377</v>
@@ -16390,16 +16870,19 @@
       <c r="AD24">
         <v>0</v>
       </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25">
         <v>31.20327</v>
@@ -16482,16 +16965,19 @@
       <c r="AD25">
         <v>1</v>
       </c>
+      <c r="AE25">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D26">
         <v>37.57769</v>
@@ -16574,16 +17060,19 @@
       <c r="AD26">
         <v>0</v>
       </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D27">
         <v>30.61714</v>
@@ -16666,16 +17155,19 @@
       <c r="AD27">
         <v>1</v>
       </c>
+      <c r="AE27">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D28">
         <v>39.29362</v>
@@ -16758,16 +17250,19 @@
       <c r="AD28">
         <v>1</v>
       </c>
+      <c r="AE28">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D29">
         <v>30.1534</v>
@@ -16850,16 +17345,19 @@
       <c r="AD29">
         <v>0</v>
       </c>
+      <c r="AE29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D30">
         <v>41.11981</v>
@@ -16942,16 +17440,19 @@
       <c r="AD30">
         <v>0</v>
       </c>
+      <c r="AE30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D31">
         <v>24.97411</v>
@@ -17034,16 +17535,19 @@
       <c r="AD31">
         <v>0</v>
       </c>
+      <c r="AE31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D32">
         <v>29.18251</v>
@@ -17126,16 +17630,19 @@
       <c r="AD32">
         <v>0</v>
       </c>
+      <c r="AE32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D33">
         <v>22.3193</v>
@@ -17218,16 +17725,19 @@
       <c r="AD33">
         <v>1</v>
       </c>
+      <c r="AE33">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D34">
         <v>22.1987</v>
@@ -17310,16 +17820,19 @@
       <c r="AD34">
         <v>0</v>
       </c>
+      <c r="AE34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D35">
         <v>23.6978</v>
@@ -17402,16 +17915,19 @@
       <c r="AD35">
         <v>0</v>
       </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D36">
         <v>47.7511</v>
@@ -17494,16 +18010,19 @@
       <c r="AD36">
         <v>0</v>
       </c>
+      <c r="AE36">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D37">
         <v>40.6331</v>
@@ -17586,16 +18105,19 @@
       <c r="AD37">
         <v>0</v>
       </c>
+      <c r="AE37">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D38">
         <v>36.7783</v>
@@ -17678,16 +18200,19 @@
       <c r="AD38">
         <v>0</v>
       </c>
+      <c r="AE38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D39">
         <v>34.0489</v>
@@ -17770,13 +18295,16 @@
       <c r="AD39">
         <v>0</v>
       </c>
+      <c r="AE39">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:31">
       <c r="B40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D40">
         <v>35.6762</v>
@@ -17859,13 +18387,16 @@
       <c r="AD40">
         <v>0</v>
       </c>
+      <c r="AE40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:31">
       <c r="B41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D41">
         <v>13.7563</v>
@@ -17948,13 +18479,16 @@
       <c r="AD41">
         <v>0</v>
       </c>
+      <c r="AE41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:31">
       <c r="B42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D42">
         <v>37.5665</v>
@@ -18037,13 +18571,16 @@
       <c r="AD42">
         <v>0</v>
       </c>
+      <c r="AE42">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:31">
       <c r="B43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D43">
         <v>1.3521</v>
@@ -18126,13 +18663,16 @@
       <c r="AD43">
         <v>0</v>
       </c>
+      <c r="AE43">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:31">
       <c r="B44" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D44">
         <v>21.0278</v>
@@ -18215,13 +18755,16 @@
       <c r="AD44">
         <v>0</v>
       </c>
+      <c r="AE44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:31">
       <c r="B45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D45">
         <v>46.2276</v>
@@ -18304,13 +18847,16 @@
       <c r="AD45">
         <v>0</v>
       </c>
+      <c r="AE45">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:31">
       <c r="B46" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D46">
         <v>28.3949</v>
@@ -18393,13 +18939,16 @@
       <c r="AD46">
         <v>0</v>
       </c>
+      <c r="AE46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:31">
       <c r="B47" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D47">
         <v>4.2105</v>
@@ -18482,16 +19031,19 @@
       <c r="AD47">
         <v>0</v>
       </c>
+      <c r="AE47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:31">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D48">
         <v>43.6532</v>
@@ -18574,16 +19126,19 @@
       <c r="AD48">
         <v>0</v>
       </c>
+      <c r="AE48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:30">
+    <row r="49" spans="1:31">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D49">
         <v>49.2827</v>
@@ -18666,16 +19221,19 @@
       <c r="AD49">
         <v>0</v>
       </c>
+      <c r="AE49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:30">
+    <row r="50" spans="1:31">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D50">
         <v>-33.8688</v>
@@ -18758,16 +19316,19 @@
       <c r="AD50">
         <v>0</v>
       </c>
+      <c r="AE50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:30">
+    <row r="51" spans="1:31">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D51">
         <v>-37.8136</v>
@@ -18850,16 +19411,19 @@
       <c r="AD51">
         <v>0</v>
       </c>
+      <c r="AE51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:30">
+    <row r="52" spans="1:31">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D52">
         <v>-27.4698</v>
@@ -18942,13 +19506,16 @@
       <c r="AD52">
         <v>0</v>
       </c>
+      <c r="AE52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:30">
+    <row r="53" spans="1:31">
       <c r="B53" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D53">
         <v>12.5657</v>
@@ -19031,13 +19598,16 @@
       <c r="AD53">
         <v>0</v>
       </c>
+      <c r="AE53">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:30">
+    <row r="54" spans="1:31">
       <c r="B54" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54">
         <v>7.8731</v>
@@ -19120,16 +19690,19 @@
       <c r="AD54">
         <v>0</v>
       </c>
+      <c r="AE54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:30">
+    <row r="55" spans="1:31">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C55" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D55">
         <v>51.1657</v>
@@ -19212,13 +19785,16 @@
       <c r="AD55">
         <v>0</v>
       </c>
+      <c r="AE55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:30">
+    <row r="56" spans="1:31">
       <c r="B56" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D56">
         <v>61.9241</v>
@@ -19301,13 +19877,16 @@
       <c r="AD56">
         <v>0</v>
       </c>
+      <c r="AE56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:30">
+    <row r="57" spans="1:31">
       <c r="B57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D57">
         <v>23.4241</v>
@@ -19390,13 +19969,16 @@
       <c r="AD57">
         <v>0</v>
       </c>
+      <c r="AE57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:31">
       <c r="B58" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D58">
         <v>12.8797</v>
@@ -19479,13 +20061,16 @@
       <c r="AD58">
         <v>1</v>
       </c>
+      <c r="AE58">
+        <v>1</v>
+      </c>
     </row>
-    <row r="59" spans="1:30">
+    <row r="59" spans="1:31">
       <c r="B59" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D59">
         <v>20.5937</v>
@@ -19568,13 +20153,16 @@
       <c r="AD59">
         <v>0</v>
       </c>
+      <c r="AE59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:30">
+    <row r="60" spans="1:31">
       <c r="B60" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C60" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D60">
         <v>41.8719</v>
@@ -19657,13 +20245,16 @@
       <c r="AD60">
         <v>0</v>
       </c>
+      <c r="AE60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:30">
+    <row r="61" spans="1:31">
       <c r="B61" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D61">
         <v>55.3781</v>
@@ -19746,13 +20337,16 @@
       <c r="AD61">
         <v>0</v>
       </c>
+      <c r="AE61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:30">
+    <row r="62" spans="1:31">
       <c r="B62" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D62">
         <v>61.524</v>
@@ -19835,13 +20429,16 @@
       <c r="AD62">
         <v>0</v>
       </c>
+      <c r="AE62">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:30">
+    <row r="63" spans="1:31">
       <c r="B63" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D63">
         <v>60.1282</v>
@@ -19924,13 +20521,16 @@
       <c r="AD63">
         <v>0</v>
       </c>
+      <c r="AE63">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:30">
+    <row r="64" spans="1:31">
       <c r="B64" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D64">
         <v>40.4637</v>
@@ -20013,16 +20613,19 @@
       <c r="AD64">
         <v>0</v>
       </c>
+      <c r="AE64">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:30">
+    <row r="65" spans="1:31">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D65">
         <v>-34.9285</v>
@@ -20105,16 +20708,19 @@
       <c r="AD65">
         <v>0</v>
       </c>
+      <c r="AE65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:30">
+    <row r="66" spans="1:31">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D66">
         <v>42.3601</v>
@@ -20197,13 +20803,16 @@
       <c r="AD66">
         <v>0</v>
       </c>
+      <c r="AE66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:30">
+    <row r="67" spans="1:31">
       <c r="B67" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D67">
         <v>50.5039</v>
@@ -20286,16 +20895,19 @@
       <c r="AD67">
         <v>0</v>
       </c>
+      <c r="AE67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:30">
+    <row r="68" spans="1:31">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D68">
         <v>43.0731</v>
@@ -20376,6 +20988,9 @@
         <v>0</v>
       </c>
       <c r="AD68">
+        <v>0</v>
+      </c>
+      <c r="AE68">
         <v>0</v>
       </c>
     </row>

</xml_diff>